<commit_message>
Now fully up to date with Word Doc.
</commit_message>
<xml_diff>
--- a/Tables/Top.5.piRNA.cluster.exp.xlsx
+++ b/Tables/Top.5.piRNA.cluster.exp.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,8 +168,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -221,12 +227,25 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -243,61 +262,21 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -325,6 +304,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -340,7 +326,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -357,32 +342,59 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -399,11 +411,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E10" headerRowCount="0" totalsRowShown="0" dataDxfId="10">
   <tableColumns count="5">
-    <tableColumn id="1" name="Cluster name" headerRowDxfId="0" dataDxfId="9"/>
-    <tableColumn id="2" name="Matched Cluster" headerRowDxfId="1" dataDxfId="8"/>
-    <tableColumn id="3" name="Unique-mapping piRNAs @ wt.14dpp" headerRowDxfId="2" dataDxfId="7"/>
-    <tableColumn id="4" name="Fraction of pachytene piRNAs" headerRowDxfId="3" dataDxfId="6"/>
-    <tableColumn id="5" name="Cumulative sum of pachytene piRNAs" headerRowDxfId="4" dataDxfId="5"/>
+    <tableColumn id="1" name="Cluster name" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="2" name="Matched Cluster" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="3" name="Unique-mapping piRNAs @ wt.14dpp" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="4" name="Fraction of pachytene piRNAs" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="5" name="Cumulative sum of pachytene piRNAs" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -733,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>